<commit_message>
Microbiome minor update and work on ccdtemplate
</commit_message>
<xml_diff>
--- a/SpecimenCollectionForm/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
+++ b/SpecimenCollectionForm/SpecimenCollectionForm/DB and Documents/Specimen Collection- Endline Parasite.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questions!$V$1:$V$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questions!$V$1:$V$57</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="238">
   <si>
     <t>SLNo</t>
   </si>
@@ -800,6 +800,15 @@
   </si>
   <si>
     <t>6.b Is the person you are collecting specimens from the same person that the Day1 team enrolled?</t>
+  </si>
+  <si>
+    <t>q3b</t>
+  </si>
+  <si>
+    <t>3b.Is this the STH 14-day visit</t>
+  </si>
+  <si>
+    <t>3.L GUv wK GmwUGBP 14-w`b wfwRU?</t>
   </si>
 </sst>
 </file>
@@ -1698,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DK441"/>
+  <dimension ref="A1:DK442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1955,7 +1964,7 @@
       </c>
       <c r="U3" s="39"/>
       <c r="V3" s="22" t="str">
-        <f t="shared" ref="V3:V34" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
+        <f t="shared" ref="V3:V35" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'dataid','frmdataid', 'tblMainQues','1-2.K¬v÷vi AvBwW I gv‡qi  AvBwW','1-2.Cluster ID and  Mother ID ','','q3','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
@@ -1979,7 +1988,7 @@
         <v>38</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>32</v>
+        <v>235</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -2002,40 +2011,31 @@
       <c r="U4" s="39"/>
       <c r="V4" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'q3','frmcombobox', 'tblMainQues','3.bgybv msMÖnKvixi AvBwW I bvg (ZvwjKv †_‡K GKRb‡K wbev©Pb Kiæb) ','3. MT ID and name (select one)  ','','q4','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:115" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'q3','frmcombobox', 'tblMainQues','3.bgybv msMÖnKvixi AvBwW I bvg (ZvwjKv †_‡K GKRb‡K wbev©Pb Kiæb) ','3. MT ID and name (select one)  ','','q3b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:115" s="39" customFormat="1" ht="90">
       <c r="A5" s="29">
         <v>4</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>32</v>
+        <v>235</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>228</v>
+      <c r="E5" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>236</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
+        <v>32</v>
+      </c>
       <c r="R5" s="39" t="s">
         <v>125</v>
       </c>
@@ -2045,33 +2045,32 @@
       <c r="T5" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U5" s="39"/>
       <c r="V5" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'q4','frmdate', 'tblMainQues','4.bgybv msMÖ‡ni ZvwiL ','4. Date of sample collection ','','q5','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:115" ht="94.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'q3b','frmsinglechoice', 'tblMainQues','3.L GUv wK GmwUGBP 14-w`b wfwRU?','3b.Is this the STH 14-day visit','','q4','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:115" ht="90.75">
       <c r="A6" s="29">
         <v>5</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="27" t="s">
-        <v>40</v>
+      <c r="E6" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>158</v>
+        <v>34</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -2094,30 +2093,30 @@
       <c r="U6" s="39"/>
       <c r="V6" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'q5','frmmultiplechoice', 'tblMainQues','5.†h wkï †_‡K bgybv msMÖ‡ni Rb¨ cÖ_g w`b ÷zj K‡›UBbvi †`Iqv n‡q‡Q Zvi AvBwW wbev©Pb Kiæb (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','5. Select which children have been given stool container on Day1 (select all that apply)','','q6','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:115" ht="99">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'q4','frmdate', 'tblMainQues','4.bgybv msMÖ‡ni ZvwiL ','4. Date of sample collection ','','q5','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:115" ht="94.5">
       <c r="A7" s="29">
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>158</v>
+        <v>34</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>168</v>
+      <c r="E7" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>169</v>
+        <v>41</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2140,31 +2139,40 @@
       <c r="U7" s="39"/>
       <c r="V7" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'q6','frmcombobox', 'tblMainQues','6.‡hme e¨w³i KvQ †_‡K GLb bgybv msMÖn Kiv n‡”Q Zv‡`i cÖ‡Z¨‡Ki Avjv`v Avjv`v AvBwW wbev©Pb Kiæb  (GKwU AvBwW wbev©Pb Kiæb)    ','6.Select the ID of the individual whose sample you are collecting now (select one)','','q7','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:115" s="39" customFormat="1" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'q5','frmmultiplechoice', 'tblMainQues','5.†h wkï †_‡K bgybv msMÖ‡ni Rb¨ cÖ_g w`b ÷zj K‡›UBbvi †`Iqv n‡q‡Q Zvi AvBwW wbev©Pb Kiæb (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','5. Select which children have been given stool container on Day1 (select all that apply)','','q6','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:115" ht="99">
       <c r="A8" s="29">
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>142</v>
+        <v>27</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>42</v>
       </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
       <c r="R8" s="39" t="s">
         <v>125</v>
       </c>
@@ -2174,42 +2182,34 @@
       <c r="T8" s="39" t="s">
         <v>126</v>
       </c>
+      <c r="U8" s="39"/>
       <c r="V8" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'q6b','frmsinglechoice', 'tblMainQuesL','6.L eZ©gv‡b †h e¨w³i KvQ †_‡K Avcwb bgybv msMÖn Ki‡Qb wZwb †W-1 wU‡gi ZvwjKvfz³ GKB e¨w³wK?','6.b Is the person you are collecting specimens from the same person that the Day1 team enrolled?','','q7','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:115" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'q6','frmcombobox', 'tblMainQues','6.‡hme e¨w³i KvQ †_‡K GLb bgybv msMÖn Kiv n‡”Q Zv‡`i cÖ‡Z¨‡Ki Avjv`v Avjv`v AvBwW wbev©Pb Kiæb  (GKwU AvBwW wbev©Pb Kiæb)    ','6.Select the ID of the individual whose sample you are collecting now (select one)','','q7','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:115" s="39" customFormat="1" ht="90">
       <c r="A9" s="29">
         <v>8</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>48</v>
+        <v>232</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>230</v>
+      <c r="E9" s="31" t="s">
+        <v>233</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
+        <v>42</v>
+      </c>
       <c r="R9" s="39" t="s">
         <v>125</v>
       </c>
@@ -2219,34 +2219,42 @@
       <c r="T9" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U9" s="39"/>
       <c r="V9" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'q7','frmtext', 'tblMainQuesL','7.AvBwW Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)','7.Enter the name of the individual (check against your ID list from Day1 team)','','q8','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:115" s="39" customFormat="1" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'q6b','frmsinglechoice', 'tblMainQuesL','6.L eZ©gv‡b †h e¨w³i KvQ †_‡K Avcwb bgybv msMÖn Ki‡Qb wZwb †W-1 wU‡gi ZvwjKvfz³ GKB e¨w³wK?','6.b Is the person you are collecting specimens from the same person that the Day1 team enrolled?','','q7','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:115" ht="90">
       <c r="A10" s="29">
         <v>9</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>178</v>
+      <c r="E10" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>170</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
       <c r="R10" s="39" t="s">
         <v>125</v>
       </c>
@@ -2256,42 +2264,34 @@
       <c r="T10" s="39" t="s">
         <v>126</v>
       </c>
+      <c r="U10" s="39"/>
       <c r="V10" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q8','frmsinglechoice', 'tblMainQuesL','8.Avcwb wK GLb D³ e¨w³ †_‡K cvqLvbv ev i‡³i bgybv msMÖn Ki‡eb?','8.Are you collecting stool or bloodfrom this person right now?','','q9','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:115" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q7','frmtext', 'tblMainQuesL','7.AvBwW Abyhvqx cÖ‡Z¨K e¨w³i bvg wjLyb ( †W-1 wUg †_‡K cÖvß AvBwW ZvwjKvi mv‡_ D³ AvBwW¸‡jv wgwj‡q wbb|)','7.Enter the name of the individual (check against your ID list from Day1 team)','','q8','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:115" s="39" customFormat="1" ht="90.75">
       <c r="A11" s="29">
         <v>10</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>51</v>
+        <v>142</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>178</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
+        <v>49</v>
+      </c>
       <c r="R11" s="39" t="s">
         <v>125</v>
       </c>
@@ -2301,18 +2301,17 @@
       <c r="T11" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U11" s="39"/>
       <c r="V11" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('10', 'q9','frmsinglechoice', 'tblMainQuesL2','9.D³ e¨w³ †_‡K gj/cvqLvbvi bgybv msMÖn Kiv n‡q‡Q wK?','9.Has a stool sample been collected from this individual?','','q10','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:115" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('10', 'q8','frmsinglechoice', 'tblMainQuesL','8.Avcwb wK GLb D³ e¨w³ †_‡K cvqLvbv ev i‡³i bgybv msMÖn Ki‡eb?','8.Are you collecting stool or bloodfrom this person right now?','','q9','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:115" ht="90.75">
       <c r="A12" s="29">
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>46</v>
@@ -2320,14 +2319,14 @@
       <c r="D12" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E12" s="27" t="s">
-        <v>54</v>
+      <c r="E12" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>159</v>
+        <v>53</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -2350,31 +2349,40 @@
       <c r="U12" s="39"/>
       <c r="V12" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('11', 'q10','frmsinglechoice', 'tblMainQuesL2','10.‡Kb cvqLvbvi bgybv msMÖn Kiv hvqwb?','10.Why has a stool sample not been collected?  ','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:115" s="39" customFormat="1" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('11', 'q9','frmsinglechoice', 'tblMainQuesL2','9.D³ e¨w³ †_‡K gj/cvqLvbvi bgybv msMÖn Kiv n‡q‡Q wK?','9.Has a stool sample been collected from this individual?','','q10','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:115" ht="90">
       <c r="A13" s="29">
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E13" s="37" t="s">
-        <v>211</v>
+      <c r="E13" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>212</v>
+        <v>55</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>159</v>
       </c>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
       <c r="R13" s="39" t="s">
         <v>125</v>
       </c>
@@ -2384,29 +2392,30 @@
       <c r="T13" s="39" t="s">
         <v>126</v>
       </c>
+      <c r="U13" s="39"/>
       <c r="V13" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('12', 'q10_other','frmtext', 'tblMainQuesL2','10.Ab¨vY¨t wbw`©ó K‡i wjLyb','10.Other: Specify','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:115" s="39" customFormat="1" ht="105">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('12', 'q10','frmsinglechoice', 'tblMainQuesL2','10.‡Kb cvqLvbvi bgybv msMÖn Kiv hvqwb?','10.Why has a stool sample not been collected?  ','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:115" s="39" customFormat="1" ht="90.75">
       <c r="A14" s="29">
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>155</v>
+        <v>210</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>220</v>
+      <c r="E14" s="37" t="s">
+        <v>211</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>159</v>
@@ -2422,40 +2431,31 @@
       </c>
       <c r="V14" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('13', 'msg01','frmmessage', 'tblMainQuesL2','D³ LvbvwU bZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Z ev †evSv‡Z msMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (*) emvb','NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:115" ht="157.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('13', 'q10_other','frmtext', 'tblMainQuesL2','10.Ab¨vY¨t wbw`©ó K‡i wjLyb','10.Other: Specify','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:115" s="39" customFormat="1" ht="105">
       <c r="A15" s="29">
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="C15" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="26" t="s">
         <v>155</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E15" s="27" t="s">
-        <v>179</v>
+      <c r="E15" s="31" t="s">
+        <v>220</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
+        <v>159</v>
+      </c>
       <c r="R15" s="39" t="s">
         <v>125</v>
       </c>
@@ -2465,33 +2465,32 @@
       <c r="T15" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U15" s="39"/>
       <c r="V15" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'msg02','frmmessage', 'tblMainQuesL2','wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| ','Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:115" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'msg01','frmmessage', 'tblMainQuesL2','D³ LvbvwU bZzb BB wm‡½j Av‡g©i AšÍ©fz³ wn‡m‡e wb‡`©k Ki‡Z ev †evSv‡Z msMÖnK…Z ÷zj K‡›UBbv‡ii wQwci Dci ZviKv wPý (*) emvb','NOTE: Mark the cap of the stool collection containersin this household with * to show that this household is in the single arm EE cohort.','','msg02','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:115" ht="157.5">
       <c r="A16" s="29">
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
+        <v>159</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>155</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>229</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -2514,7 +2513,7 @@
       <c r="U16" s="39"/>
       <c r="V16" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('15', 'q11','frmyeartomin', 'tblMainQuesL2','11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)','11.Enter the cold chain start time  (24-hr scale)','','q12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('15', 'msg02','frmmessage', 'tblMainQuesL2','wbwðZ Kiæb †h cvqLvbvi bgybv cixÿv Kivi Rb¨ Avcwb K¨v‡Uv-K¨vUR GwjKU ˆZix K‡i‡Qb Ges K¨v‡Uv-K¨vUR GwjK‡Ui Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q| ','Make sure that you have prepared a Kato-Katz aliquot for this individual and make sure that the sample ID and random ID of the barcode on the Kato-Katz aliquot match the following:','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="90">
@@ -2522,22 +2521,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>229</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -2560,7 +2559,7 @@
       <c r="U17" s="39"/>
       <c r="V17" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('16', 'q12','frmsinglechoice', 'tblMainQuesL2','12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?','12.(obs) Stool consistency','','q13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('16', 'q11','frmyeartomin', 'tblMainQuesL2','11.msM„nxZ bgybv Kyje†· ivLvi ïiæi mgqUv wjwce× Kiæb (24 N›Uv wnmv‡e)','11.Enter the cold chain start time  (24-hr scale)','','q12','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="90">
@@ -2568,7 +2567,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>46</v>
@@ -2577,13 +2576,13 @@
         <v>229</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -2606,27 +2605,27 @@
       <c r="U18" s="39"/>
       <c r="V18" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('17', 'q13','frmsinglechoice', 'tblMainQuesL2','13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?','13. (obs) Stool color','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('17', 'q12','frmsinglechoice', 'tblMainQuesL2','12.(পর্যবেক্ষন করুন) cvqLvbvi aib †Kgb?','12.(obs) Stool consistency','','q13','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="90">
       <c r="A19" s="29">
         <v>18</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>48</v>
+        <v>67</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E19" s="37" t="s">
-        <v>187</v>
+      <c r="E19" s="27" t="s">
+        <v>185</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>72</v>
@@ -2652,30 +2651,30 @@
       <c r="U19" s="39"/>
       <c r="V19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q13_other','frmtext', 'tblMainQuesL2','13.Ab¨vY¨t wbw`©ó K‡i wjLyb','13.Other: Specify','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('18', 'q13','frmsinglechoice', 'tblMainQuesL2','13.(পর্যবেক্ষন করুন) cvqLvbvi eb© wK?','13. (obs) Stool color','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="90.75">
       <c r="A20" s="29">
         <v>19</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>35</v>
+        <v>160</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E20" s="27" t="s">
-        <v>189</v>
+      <c r="E20" s="37" t="s">
+        <v>187</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -2698,29 +2697,28 @@
       <c r="U20" s="39"/>
       <c r="V20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('19', 'q14','frmmultiplechoice', 'tblMainQuesL2','14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('19', 'q13_other','frmtext', 'tblMainQuesL2','13.Ab¨vY¨t wbw`©ó K‡i wjLyb','13.Other: Specify','','q14','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="90">
       <c r="A21" s="29">
         <v>20</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>48</v>
+        <v>72</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>191</v>
+      <c r="E21" s="27" t="s">
+        <v>189</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="G21" s="36"/>
+        <v>190</v>
+      </c>
       <c r="H21" s="29" t="s">
         <v>73</v>
       </c>
@@ -2745,30 +2743,31 @@
       <c r="U21" s="39"/>
       <c r="V21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('20', 'q14_other','frmtext', 'tblMainQuesL2','14.Ab¨vY¨t wbw`©ó K‡i wjLyb','14.Other: Specify','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('20', 'q14','frmmultiplechoice', 'tblMainQuesL2','14. (পর্যবেক্ষন করুন) msM„nxZ cvqLvbvi bgybvi g‡a¨ A¯^vfvweK wKQz †`Lv †M‡Q wK? (cÖ‡hvR¨ me¸‡jv Ackb wbev©Pb Kiæb)','14.(obs) Do you see any abnormal characteristics of the collected stool sample? (Select all that apply)','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="90.75">
       <c r="A22" s="29">
         <v>21</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>46</v>
+        <v>161</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E22" s="27" t="s">
-        <v>74</v>
+      <c r="E22" s="37" t="s">
+        <v>191</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>193</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="G22" s="36"/>
       <c r="H22" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2791,7 +2790,7 @@
       <c r="U22" s="39"/>
       <c r="V22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('21', 'q15','frmsinglechoice', 'tblMainQuesL2','15.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','15.Enter the day of defecation','','q16','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('21', 'q14_other','frmtext', 'tblMainQuesL2','14.Ab¨vY¨t wbw`©ó K‡i wjLyb','14.Other: Specify','','q15','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="90">
@@ -2799,22 +2798,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>229</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>195</v>
+        <v>74</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>193</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
@@ -2837,7 +2836,7 @@
       <c r="U23" s="39"/>
       <c r="V23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('22', 'q16','frmyeartomin', 'tblMainQuesL2','16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)','16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('22', 'q15','frmsinglechoice', 'tblMainQuesL2','15.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','15.Enter the day of defecation','','q16','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="90">
@@ -2845,19 +2844,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>46</v>
+        <v>75</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>229</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>195</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>93</v>
@@ -2883,15 +2882,15 @@
       <c r="U24" s="39"/>
       <c r="V24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('23', 'q17','frmsinglechoice', 'tblMainQuesL2','17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','17.Enter the approximate time of defecation','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" s="39" customFormat="1" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('23', 'q16','frmyeartomin', 'tblMainQuesL2','16.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi mgq wjwce× Kiæb (24 N›Uv wnmv‡e, Rvwb bv n‡j 99:99 emvb)','16.Enter the time of defecation (24-hr scale, enter 99:99 for DK)','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="90">
       <c r="A25" s="29">
         <v>24</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>46</v>
@@ -2899,15 +2898,24 @@
       <c r="D25" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E25" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>199</v>
+      <c r="E25" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>197</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>166</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
       <c r="R25" s="39" t="s">
         <v>125</v>
       </c>
@@ -2917,17 +2925,18 @@
       <c r="T25" s="39" t="s">
         <v>126</v>
       </c>
+      <c r="U25" s="39"/>
       <c r="V25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('24', 'q18','frmsinglechoice', 'tblMainQuesL2','18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?','18.Was the stool collected from one defecation event or multiple defecation events?','','q19a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('24', 'q17','frmsinglechoice', 'tblMainQuesL2','17.e¨w³/wkïi cvqLvbv ev gj Z¨vM Kivi w`b wjwce× Kiæb','17.Enter the approximate time of defecation','','q18','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="39" customFormat="1" ht="90">
       <c r="A26" s="29">
         <v>25</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>46</v>
@@ -2935,24 +2944,15 @@
       <c r="D26" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E26" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>201</v>
+      <c r="E26" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>199</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
+        <v>166</v>
+      </c>
       <c r="R26" s="39" t="s">
         <v>125</v>
       </c>
@@ -2962,18 +2962,17 @@
       <c r="T26" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U26" s="39"/>
       <c r="V26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('25', 'q19a','frmsinglechoice', 'tblMainQuesL2','19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?','19.a. (obs) Is the individual wearing shoes? ','','q19b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" s="39" customFormat="1" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('25', 'q18','frmsinglechoice', 'tblMainQuesL2','18.cvqLvbvi bgybvwU GKev‡I Kiv cvqLvbv †_‡K bvwKGKvwaKevi Kiv cvqLvbv †_‡K msMÖn Kiv n‡q‡Q?','18.Was the stool collected from one defecation event or multiple defecation events?','','q19a','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="90">
       <c r="A27" s="29">
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>46</v>
@@ -2981,15 +2980,24 @@
       <c r="D27" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E27" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="F27" s="46" t="s">
-        <v>203</v>
+      <c r="E27" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>201</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>162</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
       <c r="R27" s="39" t="s">
         <v>125</v>
       </c>
@@ -2999,9 +3007,10 @@
       <c r="T27" s="39" t="s">
         <v>126</v>
       </c>
+      <c r="U27" s="39"/>
       <c r="V27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('26', 'q19b','frmsinglechoice', 'tblMainQuesL2','19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? ','19.b. Has a target child (and twin) blood sample already been collected by the EE team? ','','msg03','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('26', 'q19a','frmsinglechoice', 'tblMainQuesL2','19.K.(পর্যবেক্ষন করুন) D³ e¨w³/wkï cv‡q RyZv c‡o‡Q wK ?','19.a. (obs) Is the individual wearing shoes? ','','q19b','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="28" spans="1:22" s="39" customFormat="1" ht="90">
@@ -3009,22 +3018,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>155</v>
+        <v>46</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E28" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>164</v>
+      <c r="E28" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>203</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="R28" s="39" t="s">
         <v>125</v>
@@ -3037,40 +3046,31 @@
       </c>
       <c r="V28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('27', 'msg03','frmmessage', 'tblMainQuesL2','D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|','Do not collect a blood sample from target child (and twin) in this household','','q20','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('27', 'q19b','frmsinglechoice', 'tblMainQuesL2','19.L.BB wUg D³ Uv‡M©U wkï (Ges Uv‡M©U wkïi RgR) †_‡K i‡³i bgybv msMÖn K‡i‡Q wK ? ','19.b. Has a target child (and twin) blood sample already been collected by the EE team? ','','msg03','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="39" customFormat="1" ht="90">
       <c r="A29" s="29">
         <v>28</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E29" s="27" t="s">
-        <v>117</v>
+      <c r="E29" s="31" t="s">
+        <v>163</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
+        <v>64</v>
+      </c>
       <c r="R29" s="39" t="s">
         <v>125</v>
       </c>
@@ -3080,10 +3080,9 @@
       <c r="T29" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U29" s="39"/>
       <c r="V29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('28', 'q20','frmsinglechoice', 'tblMainQuesL2','20.D³ e¨w³/ wkï †_‡K i‡³i bgybv msMÖn Kiv n‡q‡Q wK?','20.Has a blood sample been collected from this individual?','','q21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('28', 'msg03','frmmessage', 'tblMainQuesL2','D³ Lvbvi Uv‡M©U wkï Ges Uv‡M©U wkïi RgR †_‡K i‡³i bgybv msMÖn Ki‡Z n‡ebv|','Do not collect a blood sample from target child (and twin) in this household','','q20','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="90">
@@ -3091,7 +3090,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>46</v>
@@ -3100,13 +3099,13 @@
         <v>229</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>120</v>
+        <v>214</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -3129,31 +3128,40 @@
       <c r="U30" s="39"/>
       <c r="V30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('29', 'q21','frmsinglechoice', 'tblMainQuesL2','21.‡Kb i‡³i bgybv msMÖn Kiv hvqwb?','21.Why has a blood sample not been collected?','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" s="39" customFormat="1" ht="90.75">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('29', 'q20','frmsinglechoice', 'tblMainQuesL2','20.D³ e¨w³/ wkï †_‡K i‡³i bgybv msMÖn Kiv n‡q‡Q wK?','20.Has a blood sample been collected from this individual?','','q21','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="90">
       <c r="A31" s="29">
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>48</v>
+        <v>116</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E31" s="37" t="s">
-        <v>204</v>
+      <c r="E31" s="27" t="s">
+        <v>119</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>118</v>
       </c>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
       <c r="R31" s="39" t="s">
         <v>125</v>
       </c>
@@ -3163,42 +3171,34 @@
       <c r="T31" s="39" t="s">
         <v>126</v>
       </c>
+      <c r="U31" s="39"/>
       <c r="V31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('30', 'q21_other','frmtext', 'tblMainQuesL2','21.Ab¨vY¨t wbw`©ó K‡i wjLyb','21.Other: Specify','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('30', 'q21','frmsinglechoice', 'tblMainQuesL2','21.‡Kb i‡³i bgybv msMÖn Kiv hvqwb?','21.Why has a blood sample not been collected?','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="39" customFormat="1" ht="90.75">
       <c r="A32" s="29">
         <v>31</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E32" s="27" t="s">
-        <v>231</v>
+      <c r="E32" s="37" t="s">
+        <v>204</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
+        <v>118</v>
+      </c>
       <c r="R32" s="39" t="s">
         <v>125</v>
       </c>
@@ -3208,33 +3208,32 @@
       <c r="T32" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="U32" s="39"/>
       <c r="V32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('31', 'q22','frmnumeric', 'tblMainQuesL2','22. A¨vwbwgqv †U‡÷i djvdj wjLyb. di‡gU: `yB wWwRU Gi ci `kwg‡Ki ci GK wWwRU','22.Enter the result of the anemia test. __ __. __ g/dL','','msg04','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="115.5">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('31', 'q21_other','frmtext', 'tblMainQuesL2','21.Ab¨vY¨t wbw`©ó K‡i wjLyb','21.Other: Specify','','q22','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="90">
       <c r="A33" s="29">
         <v>32</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E33" s="31" t="s">
-        <v>207</v>
+      <c r="E33" s="27" t="s">
+        <v>231</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="I33"/>
       <c r="J33"/>
@@ -3257,29 +3256,31 @@
       <c r="U33" s="39"/>
       <c r="V33" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('32', 'msg04','frmmessage', 'tblMainQuesL2','wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|','Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:','','q23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="90">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('32', 'q22','frmnumeric', 'tblMainQuesL2','22. A¨vwbwgqv †U‡÷i djvdj wjLyb. di‡gU: `yB wWwRU Gi ci `kwg‡Ki ci GK wWwRU','22.Enter the result of the anemia test. __ __. __ g/dL','','msg04','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="115.5">
       <c r="A34" s="29">
         <v>33</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="E34" s="27" t="s">
-        <v>122</v>
+      <c r="E34" s="31" t="s">
+        <v>207</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="H34" s="29"/>
+        <v>208</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>121</v>
+      </c>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -3301,26 +3302,52 @@
       <c r="U34" s="39"/>
       <c r="V34" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('33', 'q23','frmnumeric', 'tblMainQuesL2','23.wdëvi †ccv‡i i‡³i Kq‡dvUv bgybv msMÖn Kiv n‡q‡Q Zvi msL¨v wjLyb (msL¨v 1 †_‡K 6 Gi g‡a¨ n‡e)','23.Enter the number of spots filled (has to be between 1 and 6)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="E46" s="25"/>
-      <c r="H46" s="29"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46"/>
-      <c r="S46"/>
-      <c r="T46"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('33', 'msg04','frmmessage', 'tblMainQuesL2','wbwðZ Kiæb eøvW ¯úU wdëvi †ccv‡ii Mv‡q jvMv‡bv evi‡Kv‡Wi m¨v¤új AvBwW I †ibWg AvBwW mv‡_ wb‡b¥v³ m¨v¤új AvBwW I ‡ibWg AvBwW ûeû wgj Av‡Q|','Make sure that the sample ID and random ID of the barcode on the blood spot filter paper match the following:','','q23','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="90">
+      <c r="A35" s="29">
+        <v>34</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="29"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="S35" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="T35" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="U35" s="39"/>
+      <c r="V35" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('34', 'q23','frmnumeric', 'tblMainQuesL2','23.wdëvi †ccv‡i i‡³i Kq‡dvUv bgybv msMÖn Kiv n‡q‡Q Zvi msL¨v wjLyb (msL¨v 1 †_‡K 6 Gi g‡a¨ n‡e)','23.Enter the number of spots filled (has to be between 1 and 6)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
     </row>
     <row r="47" spans="1:22">
       <c r="A47" s="29"/>
@@ -10415,7 +10442,25 @@
       <c r="T440"/>
     </row>
     <row r="441" spans="1:20">
+      <c r="A441" s="29"/>
+      <c r="B441" s="29"/>
       <c r="E441" s="25"/>
+      <c r="H441" s="29"/>
+      <c r="I441"/>
+      <c r="J441"/>
+      <c r="K441"/>
+      <c r="L441"/>
+      <c r="M441"/>
+      <c r="N441"/>
+      <c r="O441"/>
+      <c r="P441"/>
+      <c r="Q441"/>
+      <c r="R441"/>
+      <c r="S441"/>
+      <c r="T441"/>
+    </row>
+    <row r="442" spans="1:20">
+      <c r="E442" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10425,10 +10470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1265"/>
+  <dimension ref="A1:G1267"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G62"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -10504,71 +10549,73 @@
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="22" t="str">
-        <f t="shared" ref="G3:G62" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;D3&amp;"','" &amp;C3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
+        <f t="shared" ref="G3:G64" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;D3&amp;"','" &amp;C3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','qSpil', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A4" s="39">
         <v>3</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4">
+      <c r="B4" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="39">
         <v>1</v>
       </c>
+      <c r="F4" s="29"/>
       <c r="G4" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('3','q5_1', '1.T1 Target child (parasite cohort)','1.Uv‡M©U wkï 1 (c¨vivmvBU †Kvn©U)','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('3','q3b', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A5" s="39">
         <v>4</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>134</v>
+      <c r="B5" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="E5" s="39">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F5" s="29"/>
       <c r="G5" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','q5_2', '2.T2 Target child twin (parasite cohort)','2.Uv‡M©U wkï 2 (RgR) (c¨vivmvBU †Kvn©U)','1','');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','q3b', '2.No  ','2.bv','2','');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="39">
         <v>5</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="39">
+        <v>127</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
       <c r="G6" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('5','q5_3', '3.C1 18-27 months baseline child (parasite cohort)','3.18-27 gv‡mi ‡eRjvBb wkï (c¨vivmvBU †Kvn©U)','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('5','q5_1', '1.T1 Target child (parasite cohort)','1.Uv‡M©U wkï 1 (c¨vivmvBU †Kvn©U)','1','');</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10576,20 +10623,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="41">
+        <v>128</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="39">
         <v>1</v>
       </c>
       <c r="G7" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('6','q5_4', '4.O1 5-12 yr old child 1 (parasite cohort)','4.5-12 eQi eq‡mi wkï (c¨vivmvBU †Kvn©U)]','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('6','q5_2', '2.T2 Target child twin (parasite cohort)','2.Uv‡M©U wkï 2 (RgR) (c¨vivmvBU †Kvn©U)','1','');</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10597,20 +10644,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="41">
+        <v>138</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="39">
         <v>1</v>
       </c>
       <c r="G8" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('7','q5_5', '5.A1 15+ individual 1 (STH cohort)','5.15 eQ‡ii AwaK eq‡mi wkï (GmwUGBP †Kvn©U)','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('7','q5_3', '3.C1 18-27 months baseline child (parasite cohort)','3.18-27 gv‡mi ‡eRjvBb wkï (c¨vivmvBU †Kvn©U)','1','');</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10618,70 +10665,70 @@
         <v>8</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>149</v>
+        <v>139</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>136</v>
       </c>
       <c r="E9" s="41">
         <v>1</v>
       </c>
       <c r="G9" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('8','q5_6', '6.S1 Spillover child (spillover cohort) ','6.w¯újIfvi wkï (w¯újIfvi †Kvn©U)','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('8','q5_4', '4.O1 5-12 yr old child 1 (parasite cohort)','4.5-12 eQi eq‡mi wkï (c¨vivmvBU †Kvn©U)]','1','');</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A10" s="39">
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10" s="39">
+      <c r="B10" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="41">
         <v>1</v>
       </c>
       <c r="G10" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('9','q6b', '1.Yes ','1.n¨v','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('9','q5_5', '5.A1 15+ individual 1 (STH cohort)','5.15 eQ‡ii AwaK eq‡mi wkï (GmwUGBP †Kvn©U)','1','');</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A11" s="39">
         <v>10</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="39">
-        <v>2</v>
+      <c r="B11" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="41">
+        <v>1</v>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('10','q6b', '2.No  ','2.bv','2','');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('10','q5_6', '6.S1 Spillover child (spillover cohort) ','6.w¯újIfvi wkï (w¯újIfvi †Kvn©U)','1','');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A12" s="39">
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>43</v>
+        <v>232</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>44</v>
@@ -10689,20 +10736,20 @@
       <c r="D12" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="39">
         <v>1</v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('11','q6_2', '1.Yes ','1.n¨v','1','');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('11','q6b', '1.Yes ','1.n¨v','1','');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A13" s="39">
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>43</v>
+        <v>232</v>
       </c>
       <c r="C13" s="43" t="s">
         <v>45</v>
@@ -10710,54 +10757,54 @@
       <c r="D13" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="39">
         <v>2</v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('12','q6_2', '2.No  ','2.bv','2','');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('12','q6b', '2.No  ','2.bv','2','');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" s="39">
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="39">
+        <v>43</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="33">
         <v>1</v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('13','q6', 'T1','T1','1','');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('13','q6_2', '1.Yes ','1.n¨v','1','');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="39">
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" s="39">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="33">
+        <v>2</v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('14','q6', 'T2','T2','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('14','q6_2', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10767,18 +10814,18 @@
       <c r="B16" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>147</v>
+      <c r="C16" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>145</v>
       </c>
       <c r="E16" s="39">
         <v>1</v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('15','q6', 'C1','C1','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('15','q6', 'T1','T1','1','');</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10788,18 +10835,18 @@
       <c r="B17" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="41">
+      <c r="C17" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="39">
         <v>1</v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('16','q6', 'O1','O1','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('16','q6', 'T2','T2','1','');</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10809,18 +10856,18 @@
       <c r="B18" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" s="41">
+      <c r="C18" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="39">
         <v>1</v>
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('17','q6', 'A1','A1','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('17','q6', 'C1','C1','1','');</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10830,18 +10877,18 @@
       <c r="B19" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>151</v>
+      <c r="C19" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>144</v>
       </c>
       <c r="E19" s="41">
         <v>1</v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('18','q6', 'S1','S1','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('18','q6', 'O1','O1','1','');</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10849,41 +10896,41 @@
         <v>19</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>171</v>
+        <v>158</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="E20" s="41">
         <v>1</v>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('19','q8', '1.Stool','1.cvqLvbv','1','');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="39" customFormat="1" ht="30.75">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('19','q6', 'A1','A1','1','');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A21" s="39">
         <v>20</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>218</v>
+        <v>158</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>151</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>219</v>
+        <v>151</v>
       </c>
       <c r="E21" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('20','q8', '2.Stool and blood','2.cvqLvbv + i‡³i bgybv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('20','q6', 'S1','S1','1','');</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10894,63 +10941,59 @@
         <v>47</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>217</v>
+        <v>171</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="E22" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('21','q8', '3.Blood','3.i‡³i bgybv','3','');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('21','q8', '1.Stool','1.cvqLvbv','1','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="39" customFormat="1" ht="30.75">
       <c r="A23" s="39">
         <v>22</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="34">
-        <v>1</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>159</v>
+      <c r="B23" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="E23" s="41">
+        <v>2</v>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('22','q9', '1.Yes ','1.n¨v','1','msg02');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('22','q8', '2.Stool and blood','2.cvqLvbv + i‡³i bgybv','2','');</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A24" s="39">
         <v>23</v>
       </c>
-      <c r="B24" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="34">
-        <v>2</v>
-      </c>
-      <c r="F24"/>
+      <c r="B24" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="41">
+        <v>3</v>
+      </c>
       <c r="G24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('23','q9', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('23','q8', '3.Blood','3.i‡³i bgybv','3','');</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10958,21 +11001,23 @@
         <v>24</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25">
+        <v>49</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="34">
         <v>1</v>
       </c>
-      <c r="F25" s="34"/>
+      <c r="F25" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="G25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('24','q10', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('24','q9', '1.Yes ','1.n¨v','1','msg02');</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="39" customFormat="1" ht="30">
@@ -10980,21 +11025,21 @@
         <v>25</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26">
+        <v>49</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="34">
         <v>2</v>
       </c>
-      <c r="F26" s="34"/>
+      <c r="F26"/>
       <c r="G26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('25','q10', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('25','q9', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11005,18 +11050,18 @@
         <v>53</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('26','q10', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('26','q10', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11026,63 +11071,65 @@
       <c r="B28" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="42" t="s">
-        <v>63</v>
+      <c r="C28" s="40" t="s">
+        <v>58</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>210</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F28" s="34"/>
       <c r="G28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('27','q10', '4.Other','4.Ab¨vb¨','4','q10_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('27','q10', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A29" s="39">
         <v>28</v>
       </c>
-      <c r="B29" s="29" t="s">
-        <v>65</v>
+      <c r="B29" s="34" t="s">
+        <v>53</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>87</v>
+        <v>60</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="E29">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F29" s="34"/>
       <c r="G29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('28','q12', '1.Unformed, watery','1.AmsMwVZ, Zij','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('28','q10', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A30" s="39">
         <v>29</v>
       </c>
-      <c r="B30" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>89</v>
+      <c r="B30" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>210</v>
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('29','q12', '2.Formed, soft, moist','2.msMwVZ, big, ‡fRv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('29','q10', '4.Other','4.Ab¨vb¨','4','q10_other');</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11093,17 +11140,17 @@
         <v>65</v>
       </c>
       <c r="C31" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>91</v>
+        <v>86</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>87</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('30','q12', '3.Formed, hard, dry','3.msMwVZ, k³, ïKbv','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('30','q12', '1.Unformed, watery','1.AmsMwVZ, Zij','1','');</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11111,21 +11158,20 @@
         <v>31</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32"/>
+        <v>2</v>
+      </c>
       <c r="G32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('31','q13', '1.Yellow','1.njy`','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('31','q12', '2.Formed, soft, moist','2.msMwVZ, big, ‡fRv','2','');</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11133,21 +11179,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>97</v>
+        <v>90</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33"/>
+        <v>3</v>
+      </c>
       <c r="G33" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('32','q13', '2.Brown','2.ev`vgx','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('32','q12', '3.Formed, hard, dry','3.msMwVZ, k³, ïKbv','3','');</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11158,18 +11203,18 @@
         <v>67</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F34"/>
       <c r="G34" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('33','q13', '3.Black','3.Kv‡jv','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('33','q13', '1.Yellow','1.njy`','1','');</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11180,18 +11225,18 @@
         <v>67</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35"/>
       <c r="G35" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('34','q13', '4.Green','4.meyR','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('34','q13', '2.Brown','2.ev`vgx','2','');</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11202,18 +11247,18 @@
         <v>67</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36"/>
       <c r="G36" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('35','q13', '5.White/grey','5.mv`v/aymi','5','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('35','q13', '3.Black','3.Kv‡jv','3','');</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11224,20 +11269,18 @@
         <v>67</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E37">
-        <v>6</v>
-      </c>
-      <c r="F37" s="39" t="s">
-        <v>160</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F37"/>
       <c r="G37" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('36','q13', '6.Other: Specify','6.Ab¨vY¨t wbw`©ó K‡i wjLyb','6','q13_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('36','q13', '4.Green','4.meyR','4','');</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11245,21 +11288,21 @@
         <v>37</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>223</v>
+        <v>67</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F38"/>
       <c r="G38" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('37','q14_1', '1.No abnormal characteristics','1.A¯^vfvweK wKQz †`Lv hvqwb','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('37','q13', '5.White/grey','5.mv`v/aymi','5','');</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11267,21 +11310,23 @@
         <v>38</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>224</v>
+        <v>67</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39"/>
+        <v>6</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>160</v>
+      </c>
       <c r="G39" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','q14_2', '2.Mucus','2.†kø®§v ev K‡di gZ wcQj g‡b n‡q‡Q','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','q13', '6.Other: Specify','6.Ab¨vY¨t wbw`©ó K‡i wjLyb','6','q13_other');</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11289,13 +11334,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -11303,7 +11348,7 @@
       <c r="F40"/>
       <c r="G40" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('39','q14_3', '3.Blood','3.gj/cvqLvbvi mv‡_ i³ †`Lv †M‡Q','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('39','q14_1', '1.No abnormal characteristics','1.A¯^vfvweK wKQz †`Lv hvqwb','1','');</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11311,13 +11356,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -11325,7 +11370,7 @@
       <c r="F41"/>
       <c r="G41" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('40','q14_4', '4.Worms','4.K„wg †`Lv †M‡Q','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('40','q14_2', '2.Mucus','2.†kø®§v ev K‡di gZ wcQj g‡b n‡q‡Q','1','');</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11333,23 +11378,21 @@
         <v>41</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42" s="39" t="s">
-        <v>161</v>
-      </c>
+      <c r="F42"/>
       <c r="G42" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('41','q14_5', '5.Other: Specify','5.Ab¨vY¨t wbw`©ó K‡i wjLyb','1','q14_other');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('41','q14_3', '3.Blood','3.gj/cvqLvbvi mv‡_ i³ †`Lv †M‡Q','1','');</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="39" customFormat="1" ht="30">
@@ -11357,62 +11400,66 @@
         <v>42</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>73</v>
+        <v>226</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
+      <c r="F43"/>
       <c r="G43" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('42','q15', '1.Today','1.AvR','1','');</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('42','q14_4', '4.Worms','4.K„wg †`Lv †M‡Q','1','');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A44" s="39">
         <v>43</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>73</v>
+        <v>227</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>161</v>
       </c>
       <c r="G44" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('43','q15', '2.Yesterday','2.MZKvj','2','');</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('43','q14_5', '5.Other: Specify','5.Ab¨vY¨t wbw`©ó K‡i wjLyb','1','q14_other');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A45" s="39">
         <v>44</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="G45" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('44','q17', '1.Morning','1.mKvj','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('44','q15', '1.Today','1.AvR','1','');</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30">
@@ -11420,20 +11467,20 @@
         <v>45</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
       <c r="G46" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('45','q17', '2.Noon','2.`ycyi','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('45','q15', '2.Yesterday','2.MZKvj','2','');</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30">
@@ -11444,17 +11491,17 @@
         <v>92</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D47" s="38" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G47" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('46','q17', '3.Afternoon','3.weKvj','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('46','q17', '1.Morning','1.mKvj','1','');</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30">
@@ -11465,17 +11512,17 @@
         <v>92</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G48" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('47','q17', '4.Evening','4.mÜ¨v','4','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('47','q17', '2.Noon','2.`ycyi','2','');</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30">
@@ -11486,104 +11533,104 @@
         <v>92</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G49" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('48','q17', '5.Night','5.ivZ','5','');</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('48','q17', '3.Afternoon','3.weKvj','3','');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30">
       <c r="A50" s="39">
         <v>49</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>173</v>
+        <v>82</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="39">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
       </c>
       <c r="G50" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('49','q18', '1.Single','1.GKev‡I Kiv cvqLvbv †_‡K','1','');</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('49','q17', '4.Evening','4.mÜ¨v','4','');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30">
       <c r="A51" s="39">
         <v>50</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>175</v>
+        <v>84</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="39">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
       </c>
       <c r="G51" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('50','q18', '2.Multiple','2.GKvwaKev‡I Kiv cvqLvbv †_‡K','2','');</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('50','q17', '5.Night','5.ivZ','5','');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A52" s="39">
         <v>51</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" s="43" t="s">
-        <v>44</v>
+        <v>93</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>173</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E52" s="34">
+        <v>174</v>
+      </c>
+      <c r="E52" s="39">
         <v>1</v>
       </c>
       <c r="G52" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('51','q19a', '1.Yes ','1.n¨v','1','');</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('51','q18', '1.Single','1.GKev‡I Kiv cvqLvbv †_‡K','1','');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A53" s="39">
         <v>52</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="43" t="s">
-        <v>45</v>
+        <v>93</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>175</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E53" s="34">
+        <v>176</v>
+      </c>
+      <c r="E53" s="39">
         <v>2</v>
       </c>
       <c r="G53" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('52','q19a', '2.No  ','2.bv','2','');</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="39" customFormat="1" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('52','q18', '2.Multiple','2.GKvwaKev‡I Kiv cvqLvbv †_‡K','2','');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30">
       <c r="A54" s="39">
         <v>53</v>
       </c>
@@ -11591,17 +11638,17 @@
         <v>166</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>221</v>
+        <v>44</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="E54" s="39">
-        <v>3</v>
+        <v>152</v>
+      </c>
+      <c r="E54" s="34">
+        <v>1</v>
       </c>
       <c r="G54" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('53','q19a', '3.Could not observe','3.ch©‡eÿb Kiv m¤¢e nqwb','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('53','q19a', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30">
@@ -11609,49 +11656,49 @@
         <v>54</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="E55" s="34">
+        <v>2</v>
       </c>
       <c r="G55" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('54','q19b', '1.Yes ','1.n¨v','1','');</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('54','q19a', '2.No  ','2.bv','2','');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="39" customFormat="1" ht="30">
       <c r="A56" s="39">
         <v>55</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="E56">
-        <v>2</v>
+        <v>222</v>
+      </c>
+      <c r="E56" s="39">
+        <v>3</v>
       </c>
       <c r="G56" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('55','q19b', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('55','q19a', '3.Could not observe','3.ch©‡eÿb Kiv m¤¢e nqwb','3','');</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30">
       <c r="A57" s="39">
         <v>56</v>
       </c>
-      <c r="B57" s="36" t="s">
-        <v>64</v>
+      <c r="B57" s="29" t="s">
+        <v>167</v>
       </c>
       <c r="C57" s="43" t="s">
         <v>44</v>
@@ -11659,20 +11706,20 @@
       <c r="D57" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="E57" s="36">
+      <c r="E57">
         <v>1</v>
       </c>
       <c r="G57" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('56','q20', '1.Yes ','1.n¨v','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('56','q19b', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30">
       <c r="A58" s="39">
         <v>57</v>
       </c>
-      <c r="B58" s="36" t="s">
-        <v>64</v>
+      <c r="B58" s="29" t="s">
+        <v>167</v>
       </c>
       <c r="C58" s="43" t="s">
         <v>45</v>
@@ -11680,12 +11727,12 @@
       <c r="D58" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="E58" s="36">
+      <c r="E58">
         <v>2</v>
       </c>
       <c r="G58" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('57','q20', '2.No  ','2.bv','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('57','q19b', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="30">
@@ -11693,20 +11740,20 @@
         <v>58</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="40" t="s">
-        <v>56</v>
+        <v>64</v>
+      </c>
+      <c r="C59" s="43" t="s">
+        <v>44</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="E59" s="36">
         <v>1</v>
       </c>
       <c r="G59" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('58','q21', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('58','q20', '1.Yes ','1.n¨v','1','');</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="30">
@@ -11714,20 +11761,20 @@
         <v>59</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="40" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="C60" s="43" t="s">
+        <v>45</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
       <c r="E60" s="36">
         <v>2</v>
       </c>
       <c r="G60" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('59','q21', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('59','q20', '2.No  ','2.bv','2','');</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="30">
@@ -11738,17 +11785,17 @@
         <v>116</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E61" s="36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G61" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('60','q21', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('60','q21', '1.Subject not available','1.D³ e¨w³ Dcw¯’Z wQj bv','1','');</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="30">
@@ -11758,34 +11805,64 @@
       <c r="B62" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="C62" s="42" t="s">
-        <v>63</v>
+      <c r="C62" s="40" t="s">
+        <v>58</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E62" s="36">
-        <v>4</v>
-      </c>
-      <c r="F62" s="29" t="s">
-        <v>177</v>
+        <v>2</v>
       </c>
       <c r="G62" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('61','q21', '4.Other','4.Ab¨vb¨','4','q21_other');</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="C63" s="40"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="G63"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="C64" s="40"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="G64"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('61','q21', '2.Subject not cooperative','2.D³ e¨w³ mn‡hvwMZv K‡iwb','2','');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30">
+      <c r="A63" s="39">
+        <v>62</v>
+      </c>
+      <c r="B63" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E63" s="36">
+        <v>3</v>
+      </c>
+      <c r="G63" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('62','q21', '3.Sample not available','3.bgybv cvIqv hvqwb','3','');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30">
+      <c r="A64" s="39">
+        <v>63</v>
+      </c>
+      <c r="B64" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="36">
+        <v>4</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="G64" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('63','q21', '4.Other','4.Ab¨vb¨','4','q21_other');</v>
+      </c>
     </row>
     <row r="65" spans="3:7">
       <c r="C65" s="40"/>
@@ -18992,6 +19069,18 @@
       <c r="D1265"/>
       <c r="E1265"/>
       <c r="G1265"/>
+    </row>
+    <row r="1266" spans="3:7">
+      <c r="C1266" s="40"/>
+      <c r="D1266"/>
+      <c r="E1266"/>
+      <c r="G1266"/>
+    </row>
+    <row r="1267" spans="3:7">
+      <c r="C1267" s="40"/>
+      <c r="D1267"/>
+      <c r="E1267"/>
+      <c r="G1267"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>